<commit_message>
[Document, Modified]: Project OOAD
</commit_message>
<xml_diff>
--- a/Sơ đồ tương tác/Sơ đồ tương tác.xlsx
+++ b/Sơ đồ tương tác/Sơ đồ tương tác.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t xml:space="preserve">Login</t>
   </si>
@@ -46,7 +46,7 @@
     <t xml:space="preserve">Statistic</t>
   </si>
   <si>
-    <t xml:space="preserve">Tổng</t>
+    <t xml:space="preserve">Sum</t>
   </si>
   <si>
     <t xml:space="preserve">Trang giới thiệu
@@ -77,10 +77,6 @@
 &lt;&lt;boundary&gt;&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Login
-&lt;&lt;Control&gt;&gt;</t>
-  </si>
-  <si>
     <t xml:space="preserve">Account
 &lt;&lt;Entity&gt;&gt;</t>
   </si>
@@ -133,7 +129,7 @@
 &lt;&lt;boundary&gt;&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">UserAccount
+    <t xml:space="preserve">Account
 &lt;&lt;Control&gt;&gt;</t>
   </si>
   <si>
@@ -270,8 +266,8 @@
   </sheetPr>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:J1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J10" activeCellId="0" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="16.15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -282,7 +278,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="22.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="16.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="28.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="28.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="29.87"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="9" style="1" width="11.52"/>
   </cols>
@@ -378,7 +374,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="32.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -442,7 +438,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="4" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="32.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -546,7 +542,7 @@
         <v>16</v>
       </c>
       <c r="B9" s="4" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C9" s="4" t="n">
         <v>0</v>
@@ -564,7 +560,7 @@
         <v>0</v>
       </c>
       <c r="H9" s="4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I9" s="4" t="n">
         <v>0</v>
@@ -578,31 +574,31 @@
         <v>17</v>
       </c>
       <c r="B10" s="4" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C10" s="4" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D10" s="4" t="n">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="E10" s="4" t="n">
         <v>0</v>
       </c>
       <c r="F10" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G10" s="4" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="H10" s="4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I10" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J10" s="4" t="n">
-        <v>7</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="32.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -613,19 +609,19 @@
         <v>0</v>
       </c>
       <c r="C11" s="4" t="n">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="D11" s="4" t="n">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="E11" s="4" t="n">
         <v>0</v>
       </c>
       <c r="F11" s="4" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G11" s="4" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="H11" s="4" t="n">
         <v>0</v>
@@ -634,7 +630,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="4" t="n">
-        <v>62</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="32.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -645,7 +641,7 @@
         <v>0</v>
       </c>
       <c r="C12" s="4" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D12" s="4" t="n">
         <v>0</v>
@@ -666,7 +662,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="32.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -677,10 +673,10 @@
         <v>0</v>
       </c>
       <c r="C13" s="4" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D13" s="4" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E13" s="4" t="n">
         <v>0</v>
@@ -698,7 +694,7 @@
         <v>0</v>
       </c>
       <c r="J13" s="4" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="32.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -712,25 +708,25 @@
         <v>0</v>
       </c>
       <c r="D14" s="4" t="n">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="E14" s="4" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F14" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G14" s="4" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H14" s="4" t="n">
         <v>0</v>
       </c>
       <c r="I14" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J14" s="4" t="n">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="32.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -744,25 +740,25 @@
         <v>0</v>
       </c>
       <c r="D15" s="4" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E15" s="4" t="n">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="F15" s="4" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G15" s="4" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H15" s="4" t="n">
         <v>0</v>
       </c>
       <c r="I15" s="4" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J15" s="4" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="32.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -779,7 +775,7 @@
         <v>0</v>
       </c>
       <c r="E16" s="4" t="n">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="F16" s="4" t="n">
         <v>0</v>
@@ -794,7 +790,7 @@
         <v>0</v>
       </c>
       <c r="J16" s="4" t="n">
-        <v>17</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="32.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -811,7 +807,7 @@
         <v>0</v>
       </c>
       <c r="E17" s="4" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F17" s="4" t="n">
         <v>0</v>
@@ -826,7 +822,7 @@
         <v>0</v>
       </c>
       <c r="J17" s="4" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="32.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -843,10 +839,10 @@
         <v>0</v>
       </c>
       <c r="E18" s="4" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F18" s="4" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G18" s="4" t="n">
         <v>0</v>
@@ -858,7 +854,7 @@
         <v>0</v>
       </c>
       <c r="J18" s="4" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="32.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -878,7 +874,7 @@
         <v>0</v>
       </c>
       <c r="F19" s="4" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G19" s="4" t="n">
         <v>0</v>
@@ -890,7 +886,7 @@
         <v>0</v>
       </c>
       <c r="J19" s="4" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="32.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -910,10 +906,10 @@
         <v>0</v>
       </c>
       <c r="F20" s="4" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G20" s="4" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H20" s="4" t="n">
         <v>0</v>
@@ -945,16 +941,16 @@
         <v>0</v>
       </c>
       <c r="G21" s="4" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H21" s="4" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="I21" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J21" s="4" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="32.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -962,7 +958,7 @@
         <v>29</v>
       </c>
       <c r="B22" s="4" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C22" s="4" t="n">
         <v>0</v>
@@ -980,7 +976,7 @@
         <v>0</v>
       </c>
       <c r="H22" s="4" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="I22" s="4" t="n">
         <v>0</v>
@@ -1012,13 +1008,13 @@
         <v>0</v>
       </c>
       <c r="H23" s="4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I23" s="4" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J23" s="4" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="32.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1047,44 +1043,13 @@
         <v>0</v>
       </c>
       <c r="I24" s="4" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="J24" s="4" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="32.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B25" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C25" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D25" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E25" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F25" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G25" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H25" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="I25" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="J25" s="4" t="n">
-        <v>5</v>
-      </c>
-    </row>
+    </row>
+    <row r="25" customFormat="false" ht="32.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="26" customFormat="false" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="27" customFormat="false" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>

</xml_diff>